<commit_message>
just goofing around initially
</commit_message>
<xml_diff>
--- a/data/game.xlsx
+++ b/data/game.xlsx
@@ -14,21 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Elf</t>
+    <t>Goblin</t>
   </si>
   <si>
-    <t>Dwarf</t>
-  </si>
-  <si>
-    <t>ATK</t>
-  </si>
-  <si>
-    <t>DEF</t>
+    <t>Grick</t>
   </si>
 </sst>
 </file>
@@ -379,50 +373,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>